<commit_message>
replace low Vr diode BAT54 with BAS101s in WirelessPowerP40_Transmitter
</commit_message>
<xml_diff>
--- a/Modules/#WirelessPowerP40_Transmitter(TS61002+TS80003)/bom.xlsx
+++ b/Modules/#WirelessPowerP40_Transmitter(TS61002+TS80003)/bom.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20380"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files_of_zhangyu\Project\KICAD\Modules\#WirelessPowerP40_Transmitter(TS61002+TS80003)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Circuits\Ki\Modules\#WirelessPowerP40_Transmitter(TS61002+TS80003)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4793647E-BFE0-4B0B-AAB1-97CBDD01F198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27927E6F-A66C-4BAE-B6BD-25841F33B4C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,22 +16,11 @@
     <sheet name="WirelessPowerTransmitter P40" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="137">
   <si>
     <t>标号</t>
   </si>
@@ -298,9 +287,6 @@
   </si>
   <si>
     <t>BAT54SW</t>
-  </si>
-  <si>
-    <t>SOT-323_SC-70</t>
   </si>
   <si>
     <t>D3</t>
@@ -447,6 +433,26 @@
   </si>
   <si>
     <t>33pF 100V</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>D1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BAS101S,215</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BAS101S</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOT-323_SC-70</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOT-23</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1432,10 +1438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1488,7 +1494,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F2">
         <v>50</v>
@@ -1515,7 +1521,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F3">
         <v>50</v>
@@ -1524,7 +1530,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="2">
-        <f t="shared" ref="H3:H56" si="0">F3*G3</f>
+        <f t="shared" ref="H3:H57" si="0">F3*G3</f>
         <v>0</v>
       </c>
     </row>
@@ -1542,7 +1548,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F4">
         <v>50</v>
@@ -1569,7 +1575,7 @@
         <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F5">
         <v>50</v>
@@ -1596,7 +1602,7 @@
         <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F6">
         <v>50</v>
@@ -1617,13 +1623,13 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F7">
         <v>50</v>
@@ -1650,7 +1656,7 @@
         <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F8">
         <v>50</v>
@@ -1677,7 +1683,7 @@
         <v>10</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F9">
         <v>50</v>
@@ -1704,7 +1710,7 @@
         <v>10</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F10">
         <v>50</v>
@@ -1731,7 +1737,7 @@
         <v>10</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F11">
         <v>50</v>
@@ -1758,7 +1764,7 @@
         <v>10</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F12">
         <v>50</v>
@@ -1785,7 +1791,7 @@
         <v>10</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F13">
         <v>50</v>
@@ -1812,7 +1818,7 @@
         <v>10</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F14">
         <v>50</v>
@@ -1839,7 +1845,7 @@
         <v>10</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F15">
         <v>50</v>
@@ -1866,7 +1872,7 @@
         <v>10</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F16">
         <v>50</v>
@@ -1893,7 +1899,7 @@
         <v>10</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F17">
         <v>50</v>
@@ -1920,7 +1926,7 @@
         <v>10</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F18">
         <v>50</v>
@@ -2001,7 +2007,7 @@
         <v>10</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F21">
         <v>50</v>
@@ -2028,7 +2034,7 @@
         <v>10</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F22">
         <v>50</v>
@@ -2055,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F23">
         <v>50</v>
@@ -2076,13 +2082,13 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D24" t="s">
         <v>53</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F24">
         <v>50</v>
@@ -2109,7 +2115,7 @@
         <v>53</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F25">
         <v>50</v>
@@ -2136,7 +2142,7 @@
         <v>53</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F26">
         <v>50</v>
@@ -2163,7 +2169,7 @@
         <v>53</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F27">
         <v>50</v>
@@ -2190,7 +2196,7 @@
         <v>53</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F28">
         <v>50</v>
@@ -2217,7 +2223,7 @@
         <v>53</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F29">
         <v>50</v>
@@ -2244,7 +2250,7 @@
         <v>53</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F30">
         <v>50</v>
@@ -2271,7 +2277,7 @@
         <v>53</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F31">
         <v>50</v>
@@ -2298,7 +2304,7 @@
         <v>53</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F32">
         <v>50</v>
@@ -2352,7 +2358,7 @@
         <v>53</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F34">
         <v>50</v>
@@ -2379,7 +2385,7 @@
         <v>53</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F35">
         <v>50</v>
@@ -2406,7 +2412,7 @@
         <v>53</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F36">
         <v>50</v>
@@ -2433,7 +2439,7 @@
         <v>53</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F37">
         <v>50</v>
@@ -2460,7 +2466,7 @@
         <v>53</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F38">
         <v>50</v>
@@ -2487,7 +2493,7 @@
         <v>53</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F39">
         <v>50</v>
@@ -2508,13 +2514,13 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D40" t="s">
         <v>53</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F40">
         <v>50</v>
@@ -2541,7 +2547,7 @@
         <v>53</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F41">
         <v>50</v>
@@ -2562,13 +2568,13 @@
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D42" t="s">
         <v>53</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F42">
         <v>50</v>
@@ -2583,16 +2589,16 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" s="4">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
         <v>91</v>
       </c>
-      <c r="B43" s="4">
-        <v>1</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>92</v>
-      </c>
-      <c r="D43" t="s">
-        <v>93</v>
       </c>
       <c r="E43" s="1">
         <v>3015</v>
@@ -2610,19 +2616,19 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B44" s="4">
         <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D44" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F44">
         <v>50</v>
@@ -2637,19 +2643,19 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B45" s="4">
         <v>4</v>
       </c>
       <c r="C45" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D45" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F45">
         <v>50</v>
@@ -2664,19 +2670,19 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B46" s="4">
         <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D46" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F46">
         <v>50</v>
@@ -2691,19 +2697,19 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B47" s="4">
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D47" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F47">
         <v>10</v>
@@ -2718,49 +2724,49 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>90</v>
+        <v>132</v>
       </c>
       <c r="B48" s="4">
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="D48" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="F48">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="G48">
         <v>0</v>
       </c>
       <c r="H48" s="2">
-        <f>F48*G48</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B49" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>88</v>
+        <v>126</v>
       </c>
       <c r="D49" t="s">
-        <v>88</v>
+        <v>125</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>89</v>
+        <v>116</v>
       </c>
       <c r="F49">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -2772,40 +2778,43 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B50" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C50" t="s">
-        <v>96</v>
+        <v>88</v>
+      </c>
+      <c r="D50" t="s">
+        <v>88</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>97</v>
+        <v>135</v>
       </c>
       <c r="F50">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G50">
         <v>0</v>
       </c>
       <c r="H50" s="2">
-        <f t="shared" si="0"/>
+        <f>F50*G50</f>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B51" s="4">
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F51">
         <v>1</v>
@@ -2820,16 +2829,16 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B52" s="4">
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="F52">
         <v>1</v>
@@ -2844,16 +2853,16 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B53" s="4">
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="F53">
         <v>1</v>
@@ -2868,16 +2877,16 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B54" s="4">
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F54">
         <v>1</v>
@@ -2892,16 +2901,16 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B55" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F55">
         <v>1</v>
@@ -2916,24 +2925,48 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>108</v>
+      </c>
+      <c r="B56" s="4">
+        <v>2</v>
+      </c>
+      <c r="C56" t="s">
+        <v>109</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F56">
+        <v>1</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>111</v>
+      </c>
+      <c r="B57" s="4">
+        <v>1</v>
+      </c>
+      <c r="C57" t="s">
         <v>112</v>
       </c>
-      <c r="B56" s="4">
-        <v>1</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="E57" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E56" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F56">
-        <v>1</v>
-      </c>
-      <c r="G56">
-        <v>0</v>
-      </c>
-      <c r="H56" s="2">
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>

</xml_diff>